<commit_message>
Update MIMXRT1064 MCU Module  - BOM.xlsx
</commit_message>
<xml_diff>
--- a/DOCUMENTS/MIMXRT1064 MCU Module  - BOM.xlsx
+++ b/DOCUMENTS/MIMXRT1064 MCU Module  - BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32470\Documents\GitHub\MIMXRT1064-MCU-Module\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32470\Documents\GitHub\MIMXRT1064-MCU-Module\DOCUMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39FC3E6-82D4-4A85-8A89-11A08E833775}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E1DCF2-F595-4299-BD1D-26A5F7E75F67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="147">
   <si>
     <t>MIMXRT1064 MCU Module  - BOM</t>
   </si>
@@ -88,9 +88,6 @@
     <t>0603</t>
   </si>
   <si>
-    <t>62.5mW Thick Film Resistors ±1% 10kΩ 0402 Chip Resistor</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
   </si>
   <si>
     <t>7272300</t>
-  </si>
-  <si>
-    <t>62.5mW Thick Film Resistors ±5%2,2MΩ 0402 Chip Resistor</t>
   </si>
   <si>
     <t>2,2M</t>
@@ -127,9 +121,6 @@
     <t>CAPACITORS</t>
   </si>
   <si>
-    <t>50V 8pF C0G 0402 Multilayer Ceramic Capacitors MLCC</t>
-  </si>
-  <si>
     <t>8pF</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
   </si>
   <si>
     <t>10225</t>
-  </si>
-  <si>
-    <t>50V 12pF ±2% 0402 Multilayer Ceramic Capacitors MLCC</t>
   </si>
   <si>
     <t>12pF</t>
@@ -169,9 +157,6 @@
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
-    <t>50V 100nF X7R ±10% 0402 Multilayer Ceramic Capacitors MLCC</t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
@@ -185,9 +170,6 @@
   </si>
   <si>
     <t>1466168</t>
-  </si>
-  <si>
-    <t>16V 220nF X7R ±10% 0402 Multilayer Ceramic Capacitors MLCC</t>
   </si>
   <si>
     <t>0.22uF</t>
@@ -205,9 +187,6 @@
     <t>120532</t>
   </si>
   <si>
-    <t>25V 1uF X5R ±10% 0402 Multilayer Ceramic Capacitors MLCC</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -223,9 +202,6 @@
     <t>1161993</t>
   </si>
   <si>
-    <t>10V 4.7uF X5R ±20% 0402 Multilayer Ceramic Capacitors MLCC</t>
-  </si>
-  <si>
     <t>4.7uF</t>
   </si>
   <si>
@@ -239,9 +215,6 @@
   </si>
   <si>
     <t>472642</t>
-  </si>
-  <si>
-    <t>10V 10uF X5R ±10% 0603 Multilayer Ceramic Capacitors MLCC</t>
   </si>
   <si>
     <t>10uF</t>
@@ -265,13 +238,7 @@
     <t>FERRITE BEAD</t>
   </si>
   <si>
-    <t>120R Ferrite Bead - 800mA - 1 - 80mΩ - ±25%</t>
-  </si>
-  <si>
     <t>120R@100MHz</t>
-  </si>
-  <si>
-    <t>MURATA</t>
   </si>
   <si>
     <t>BLM18AG121SN1D</t>
@@ -308,9 +275,6 @@
   </si>
   <si>
     <t>942</t>
-  </si>
-  <si>
-    <t>Demander c'est quel fixe, comme sur la description mouser</t>
   </si>
   <si>
     <t>DRAM 256M, 3.3V, SDRAM, 16Mx16, 166Mhz, 54 ball BGA (8mmx8mm)</t>
@@ -394,13 +358,7 @@
     <t>SMD3225-4P</t>
   </si>
   <si>
-    <t>SMD3225-4P Crystals</t>
-  </si>
-  <si>
     <t>30k</t>
-  </si>
-  <si>
-    <t>62.5mW Thick Film Resistors ±1% 30kΩ 0402 Chip Resistor</t>
   </si>
   <si>
     <t>AF0402FR-0730KL</t>
@@ -433,9 +391,6 @@
     <t>$0.2144</t>
   </si>
   <si>
-    <t>32.768kHz 7pF ±20ppm SMD3215-2P Crystals</t>
-  </si>
-  <si>
     <t>LQM21PN4R7MGRD</t>
   </si>
   <si>
@@ -443,6 +398,69 @@
   </si>
   <si>
     <t>CL10A226MQ8NRNC</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor - 10k - 62.5mW -  ±1%  - 0402</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor - 30k - 62.5mW -  ±1%  - 0402</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor - 2,2M - 62.5mW -  ±1%  - 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD MLCC - 8pF - 50V - C0G - 0.5pF - 0402 </t>
+  </si>
+  <si>
+    <t>SMD MLCC - 12pF - 50V - C0G - ±2% -  0402</t>
+  </si>
+  <si>
+    <t>SMD MLCC - 100nF - 50V - X7R - ±10% - 0402</t>
+  </si>
+  <si>
+    <t>SMD MLCC - 220nF - 16V - X7R - ±10% - 0402</t>
+  </si>
+  <si>
+    <t>SMD MLCC - 1uF - 25V - X5R - ±10% - 0402</t>
+  </si>
+  <si>
+    <t>SMD MLCC - 4.7uF - 10V - X5R - ±20% - 0402</t>
+  </si>
+  <si>
+    <t>SMD MLCC -10uF - 10V - X5R - ±10% - 0603</t>
+  </si>
+  <si>
+    <t>SMD MLCC - 22uF - 6.3V - X5R - ±20% -0603</t>
+  </si>
+  <si>
+    <t>C59461</t>
+  </si>
+  <si>
+    <t>$0.0086</t>
+  </si>
+  <si>
+    <t>$0.0765 </t>
+  </si>
+  <si>
+    <t>C86090</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>4.7uH</t>
+  </si>
+  <si>
+    <t>SMD power inductor - 4.7uH - 800mA - 0R230 -20% - 0805</t>
+  </si>
+  <si>
+    <t>SMD Ferrite - 120R - 800mA - 0.180R - 25% - SMD 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal - 24MHz - 12pF - 40R - SMD2016-4P </t>
+  </si>
+  <si>
+    <t>Crystal - 32.768kHz - 7pF - 70k - ±20ppm - SMD3215-2P</t>
   </si>
 </sst>
 </file>
@@ -624,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -648,8 +666,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -677,24 +693,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -737,6 +744,52 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,14 +1010,14 @@
   </sheetPr>
   <dimension ref="A1:V957"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C935" sqref="C935"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1"/>
   <cols>
     <col min="1" max="1" width="29.6328125" customWidth="1"/>
-    <col min="2" max="2" width="56.6328125" customWidth="1"/>
+    <col min="2" max="2" width="60.81640625" customWidth="1"/>
     <col min="3" max="3" width="19.7265625" customWidth="1"/>
     <col min="4" max="4" width="18.08984375" customWidth="1"/>
     <col min="5" max="5" width="12.6328125" customWidth="1"/>
@@ -981,22 +1034,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1059,22 +1112,22 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="13">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1087,33 +1140,33 @@
     <row r="4" spans="1:22" s="5" customFormat="1" ht="13">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M4" s="14" t="s">
         <v>20</v>
@@ -1131,36 +1184,36 @@
     <row r="5" spans="1:22" s="5" customFormat="1" ht="13">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="K5" s="12"/>
       <c r="L5" s="16" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N5" s="12"/>
       <c r="O5" s="4"/>
@@ -1173,40 +1226,40 @@
       <c r="V5" s="4"/>
     </row>
     <row r="6" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A6" s="20"/>
-      <c r="B6" s="23" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>16</v>
+      <c r="H6" s="18" t="s">
+        <v>18</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="I6" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20" t="s">
-        <v>17</v>
+      <c r="J6" s="22" t="s">
+        <v>19</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="K6" s="18"/>
+      <c r="L6" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="23" t="s">
+      <c r="M6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="20"/>
+      <c r="N6" s="18"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
@@ -1217,22 +1270,22 @@
       <c r="V6" s="9"/>
     </row>
     <row r="7" spans="1:22" ht="13">
-      <c r="A7" s="68" t="s">
-        <v>34</v>
+      <c r="A7" s="57" t="s">
+        <v>32</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1243,40 +1296,40 @@
       <c r="V7" s="1"/>
     </row>
     <row r="8" spans="1:22" ht="13">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>16</v>
+      <c r="H8" s="24" t="s">
+        <v>18</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="I8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="28" t="s">
+      <c r="J8" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="K8" s="24"/>
+      <c r="L8" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="26" t="s">
-        <v>18</v>
+      <c r="M8" s="25" t="s">
+        <v>31</v>
       </c>
-      <c r="I8" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="M8" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" s="26"/>
+      <c r="N8" s="24"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1287,40 +1340,40 @@
       <c r="V8" s="2"/>
     </row>
     <row r="9" spans="1:22" ht="13">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="31" t="s">
+      <c r="K9" s="29"/>
+      <c r="L9" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32" t="s">
-        <v>37</v>
+      <c r="M9" s="31" t="s">
+        <v>31</v>
       </c>
-      <c r="G9" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="31"/>
+      <c r="N9" s="29"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1331,40 +1384,40 @@
       <c r="V9" s="2"/>
     </row>
     <row r="10" spans="1:22" ht="13">
-      <c r="A10" s="26"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="24"/>
+      <c r="L10" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="M10" s="27" t="s">
+      <c r="M10" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="26"/>
+      <c r="N10" s="24"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -1375,40 +1428,40 @@
       <c r="V10" s="2"/>
     </row>
     <row r="11" spans="1:22" ht="13">
-      <c r="A11" s="31"/>
-      <c r="B11" s="32" t="s">
-        <v>55</v>
+      <c r="A11" s="29"/>
+      <c r="B11" s="30" t="s">
+        <v>132</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>56</v>
+      <c r="D11" s="29" t="s">
+        <v>50</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32" t="s">
-        <v>48</v>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30" t="s">
+        <v>44</v>
       </c>
-      <c r="G11" s="32" t="s">
-        <v>57</v>
+      <c r="G11" s="30" t="s">
+        <v>51</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="32" t="s">
-        <v>58</v>
+      <c r="I11" s="30" t="s">
+        <v>52</v>
       </c>
-      <c r="J11" s="34" t="s">
-        <v>59</v>
+      <c r="J11" s="32" t="s">
+        <v>53</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="35" t="s">
-        <v>60</v>
+      <c r="K11" s="29"/>
+      <c r="L11" s="33" t="s">
+        <v>54</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="M11" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="31"/>
+      <c r="N11" s="29"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -1419,40 +1472,40 @@
       <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" ht="13">
-      <c r="A12" s="26"/>
-      <c r="B12" s="28" t="s">
-        <v>61</v>
+      <c r="A12" s="24"/>
+      <c r="B12" s="26" t="s">
+        <v>133</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>62</v>
+      <c r="D12" s="24" t="s">
+        <v>55</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="28" t="s">
-        <v>48</v>
+      <c r="E12" s="24"/>
+      <c r="F12" s="26" t="s">
+        <v>44</v>
       </c>
-      <c r="G12" s="28" t="s">
-        <v>63</v>
+      <c r="G12" s="26" t="s">
+        <v>56</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="28" t="s">
-        <v>64</v>
+      <c r="I12" s="26" t="s">
+        <v>57</v>
       </c>
-      <c r="J12" s="29" t="s">
-        <v>65</v>
+      <c r="J12" s="27" t="s">
+        <v>58</v>
       </c>
-      <c r="K12" s="26"/>
-      <c r="L12" s="30" t="s">
-        <v>66</v>
+      <c r="K12" s="24"/>
+      <c r="L12" s="28" t="s">
+        <v>59</v>
       </c>
-      <c r="M12" s="27" t="s">
+      <c r="M12" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="26"/>
+      <c r="N12" s="24"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -1463,40 +1516,40 @@
       <c r="V12" s="2"/>
     </row>
     <row r="13" spans="1:22" ht="13">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32" t="s">
-        <v>67</v>
+      <c r="A13" s="29"/>
+      <c r="B13" s="30" t="s">
+        <v>134</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="31" t="s">
-        <v>68</v>
+      <c r="D13" s="29" t="s">
+        <v>60</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32" t="s">
-        <v>48</v>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30" t="s">
+        <v>44</v>
       </c>
-      <c r="G13" s="32" t="s">
-        <v>69</v>
+      <c r="G13" s="30" t="s">
+        <v>61</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="32" t="s">
-        <v>70</v>
+      <c r="I13" s="30" t="s">
+        <v>62</v>
       </c>
-      <c r="J13" s="34" t="s">
-        <v>71</v>
+      <c r="J13" s="32" t="s">
+        <v>63</v>
       </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="35" t="s">
-        <v>72</v>
+      <c r="K13" s="29"/>
+      <c r="L13" s="33" t="s">
+        <v>64</v>
       </c>
-      <c r="M13" s="33" t="s">
+      <c r="M13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="31"/>
+      <c r="N13" s="29"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -1507,40 +1560,40 @@
       <c r="V13" s="2"/>
     </row>
     <row r="14" spans="1:22" ht="13">
-      <c r="A14" s="26"/>
-      <c r="B14" s="28" t="s">
-        <v>73</v>
+      <c r="A14" s="24"/>
+      <c r="B14" s="26" t="s">
+        <v>135</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="26" t="s">
-        <v>74</v>
+      <c r="D14" s="24" t="s">
+        <v>65</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="28" t="s">
-        <v>48</v>
+      <c r="E14" s="24"/>
+      <c r="F14" s="26" t="s">
+        <v>44</v>
       </c>
-      <c r="G14" s="28" t="s">
-        <v>75</v>
+      <c r="G14" s="26" t="s">
+        <v>66</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="28" t="s">
-        <v>76</v>
+      <c r="I14" s="26" t="s">
+        <v>67</v>
       </c>
-      <c r="J14" s="29" t="s">
-        <v>77</v>
+      <c r="J14" s="27" t="s">
+        <v>68</v>
       </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="30" t="s">
-        <v>78</v>
+      <c r="K14" s="24"/>
+      <c r="L14" s="28" t="s">
+        <v>69</v>
       </c>
-      <c r="M14" s="27" t="s">
+      <c r="M14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="26"/>
+      <c r="N14" s="24"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -1550,51 +1603,67 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="13">
-      <c r="A15" s="26"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="26" t="s">
-        <v>139</v>
+    <row r="15" spans="1:22" s="72" customFormat="1" ht="13">
+      <c r="A15" s="66"/>
+      <c r="B15" s="67" t="s">
+        <v>136</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28" t="s">
-        <v>140</v>
+      <c r="C15" s="68" t="s">
+        <v>21</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
+      <c r="D15" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="66"/>
+      <c r="F15" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="69" t="s">
+        <v>137</v>
+      </c>
+      <c r="J15" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="K15" s="66"/>
+      <c r="L15" s="69">
+        <v>1692113</v>
+      </c>
+      <c r="M15" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="66"/>
+      <c r="O15" s="71"/>
+      <c r="P15" s="71"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="71"/>
+      <c r="V15" s="71"/>
     </row>
     <row r="16" spans="1:22" ht="13">
-      <c r="A16" s="68" t="s">
-        <v>79</v>
+      <c r="A16" s="57" t="s">
+        <v>70</v>
       </c>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="68"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -1604,49 +1673,67 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22" s="5" customFormat="1" ht="13">
-      <c r="A17" s="36"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36" t="s">
-        <v>138</v>
+    <row r="17" spans="1:22" s="52" customFormat="1" ht="13">
+      <c r="A17" s="34"/>
+      <c r="B17" s="43" t="s">
+        <v>143</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
+      <c r="C17" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="61" t="s">
+        <v>140</v>
+      </c>
+      <c r="J17" s="61" t="s">
+        <v>139</v>
+      </c>
+      <c r="K17" s="34"/>
+      <c r="L17" s="61">
+        <v>4343</v>
+      </c>
+      <c r="M17" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="34"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="51"/>
     </row>
     <row r="18" spans="1:22" ht="13">
-      <c r="A18" s="68" t="s">
-        <v>80</v>
+      <c r="A18" s="57" t="s">
+        <v>71</v>
       </c>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
-      <c r="N18" s="68"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -1656,67 +1743,67 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" ht="13">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26" t="s">
-        <v>81</v>
+    <row r="19" spans="1:22" s="63" customFormat="1" ht="13">
+      <c r="A19" s="59"/>
+      <c r="B19" s="59" t="s">
+        <v>144</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>82</v>
+      <c r="D19" s="59" t="s">
+        <v>72</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26" t="s">
-        <v>83</v>
+      <c r="E19" s="59"/>
+      <c r="F19" s="61" t="s">
+        <v>34</v>
       </c>
-      <c r="G19" s="26" t="s">
-        <v>84</v>
+      <c r="G19" s="59" t="s">
+        <v>73</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="H19" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="26" t="s">
-        <v>85</v>
+      <c r="I19" s="59" t="s">
+        <v>74</v>
       </c>
-      <c r="J19" s="26" t="s">
-        <v>86</v>
+      <c r="J19" s="59" t="s">
+        <v>75</v>
       </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="30" t="s">
-        <v>87</v>
+      <c r="K19" s="59"/>
+      <c r="L19" s="65" t="s">
+        <v>76</v>
       </c>
-      <c r="M19" s="27" t="s">
-        <v>33</v>
+      <c r="M19" s="60" t="s">
+        <v>31</v>
       </c>
-      <c r="N19" s="26"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="62"/>
+      <c r="U19" s="62"/>
+      <c r="V19" s="62"/>
     </row>
     <row r="20" spans="1:22" ht="13">
-      <c r="A20" s="67" t="s">
-        <v>88</v>
+      <c r="A20" s="56" t="s">
+        <v>77</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="67"/>
-      <c r="L20" s="67"/>
-      <c r="M20" s="67"/>
-      <c r="N20" s="67"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
@@ -1727,40 +1814,38 @@
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="1:22" ht="13">
-      <c r="A21" s="42"/>
-      <c r="B21" s="43" t="s">
-        <v>89</v>
+      <c r="A21" s="35"/>
+      <c r="B21" s="36" t="s">
+        <v>78</v>
       </c>
-      <c r="C21" s="28" t="s">
-        <v>90</v>
+      <c r="C21" s="26" t="s">
+        <v>79</v>
       </c>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="28" t="s">
-        <v>91</v>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="26" t="s">
+        <v>80</v>
       </c>
-      <c r="G21" s="45" t="s">
-        <v>92</v>
+      <c r="G21" s="38" t="s">
+        <v>81</v>
       </c>
-      <c r="H21" s="45" t="s">
+      <c r="H21" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="28" t="s">
-        <v>93</v>
+      <c r="I21" s="26" t="s">
+        <v>82</v>
       </c>
-      <c r="J21" s="29" t="s">
-        <v>94</v>
+      <c r="J21" s="27" t="s">
+        <v>83</v>
       </c>
-      <c r="K21" s="46"/>
-      <c r="L21" s="47" t="s">
-        <v>95</v>
+      <c r="K21" s="39"/>
+      <c r="L21" s="40" t="s">
+        <v>84</v>
       </c>
-      <c r="M21" s="47" t="s">
-        <v>33</v>
+      <c r="M21" s="40" t="s">
+        <v>31</v>
       </c>
-      <c r="N21" s="45" t="s">
-        <v>96</v>
-      </c>
+      <c r="N21" s="38"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
@@ -1770,111 +1855,111 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="1:22" s="5" customFormat="1" ht="13">
-      <c r="A22" s="39"/>
-      <c r="B22" s="48" t="s">
+    <row r="22" spans="1:22" s="6" customFormat="1" ht="13">
+      <c r="A22" s="18"/>
+      <c r="B22" s="74" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="76"/>
+      <c r="L22" s="23">
+        <v>280</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" s="18"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+    </row>
+    <row r="23" spans="1:22" s="5" customFormat="1" ht="13">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J23" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="K23" s="73"/>
+      <c r="L23" s="14">
+        <v>2304</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" s="12"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+    </row>
+    <row r="24" spans="1:22" ht="13">
+      <c r="A24" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="G22" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="J22" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="K22" s="50"/>
-      <c r="L22" s="41">
-        <v>280</v>
-      </c>
-      <c r="M22" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="N22" s="39"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-    </row>
-    <row r="23" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="K23" s="51"/>
-      <c r="L23" s="18">
-        <v>2304</v>
-      </c>
-      <c r="M23" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N23" s="17"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-    </row>
-    <row r="24" spans="1:22" ht="13">
-      <c r="A24" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="68"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="57"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
@@ -1884,85 +1969,85 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="1:22" s="63" customFormat="1" ht="13">
-      <c r="A25" s="59"/>
-      <c r="B25" s="19" t="s">
-        <v>124</v>
+    <row r="25" spans="1:22" s="52" customFormat="1" ht="13">
+      <c r="A25" s="48"/>
+      <c r="B25" s="17" t="s">
+        <v>145</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>123</v>
+      <c r="C25" s="17" t="s">
+        <v>111</v>
       </c>
-      <c r="D25" s="59" t="s">
+      <c r="D25" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="48"/>
+      <c r="F25" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="J25" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="K25" s="49"/>
+      <c r="L25" s="17">
+        <v>2955</v>
+      </c>
+      <c r="M25" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="N25" s="48"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="51"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="51"/>
+      <c r="V25" s="51"/>
+    </row>
+    <row r="26" spans="1:22" ht="14.5">
+      <c r="A26" s="45"/>
+      <c r="B26" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="45"/>
+      <c r="F26" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="J26" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="E25" s="59"/>
-      <c r="F25" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G25" s="65" t="s">
-        <v>118</v>
-      </c>
-      <c r="H25" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="J25" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="K25" s="60"/>
-      <c r="L25" s="19">
-        <v>2955</v>
-      </c>
-      <c r="M25" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="N25" s="59"/>
-      <c r="O25" s="62"/>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="62"/>
-      <c r="R25" s="62"/>
-      <c r="S25" s="62"/>
-      <c r="T25" s="62"/>
-      <c r="U25" s="62"/>
-      <c r="V25" s="62"/>
-    </row>
-    <row r="26" spans="1:22" ht="14.5">
-      <c r="A26" s="56"/>
-      <c r="B26" s="66" t="s">
-        <v>137</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="D26" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="56"/>
-      <c r="F26" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="G26" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="H26" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="J26" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="K26" s="56"/>
-      <c r="L26" s="22">
+      <c r="K26" s="45"/>
+      <c r="L26" s="20">
         <v>1441</v>
       </c>
-      <c r="M26" s="57" t="s">
-        <v>33</v>
+      <c r="M26" s="46" t="s">
+        <v>31</v>
       </c>
-      <c r="N26" s="56"/>
+      <c r="N26" s="45"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -1972,22 +2057,22 @@
       <c r="U26" s="2"/>
     </row>
     <row r="27" spans="1:22" ht="13">
-      <c r="A27" s="68" t="s">
-        <v>112</v>
+      <c r="A27" s="57" t="s">
+        <v>100</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="68"/>
-      <c r="N27" s="68"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="57"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="57"/>
+      <c r="N27" s="57"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
@@ -1998,36 +2083,36 @@
       <c r="V27" s="2"/>
     </row>
     <row r="28" spans="1:22" s="3" customFormat="1" ht="13">
-      <c r="A28" s="55"/>
-      <c r="B28" s="52" t="s">
-        <v>117</v>
+      <c r="A28" s="44"/>
+      <c r="B28" s="41" t="s">
+        <v>105</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="52" t="s">
-        <v>113</v>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="41" t="s">
+        <v>101</v>
       </c>
-      <c r="G28" s="52" t="s">
-        <v>114</v>
+      <c r="G28" s="41" t="s">
+        <v>102</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="H28" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="52" t="s">
-        <v>115</v>
+      <c r="I28" s="41" t="s">
+        <v>103</v>
       </c>
-      <c r="J28" s="53" t="s">
-        <v>116</v>
+      <c r="J28" s="42" t="s">
+        <v>104</v>
       </c>
-      <c r="K28" s="55"/>
-      <c r="L28" s="54">
+      <c r="K28" s="44"/>
+      <c r="L28" s="43">
         <v>4957</v>
       </c>
-      <c r="M28" s="27" t="s">
-        <v>33</v>
+      <c r="M28" s="25" t="s">
+        <v>31</v>
       </c>
-      <c r="N28" s="55"/>
+      <c r="N28" s="44"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>

</xml_diff>